<commit_message>
commited second in time, from second repository.
</commit_message>
<xml_diff>
--- a/Test/excel doc.xlsx
+++ b/Test/excel doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Column1</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Column6</t>
+  </si>
+  <si>
+    <t>New from second repository.</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G17"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -391,7 +394,7 @@
     <col min="2" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -410,8 +413,11 @@
       <c r="G2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
       <c r="B3">
         <v>1</v>
       </c>
@@ -431,7 +437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:9">
       <c r="B4">
         <v>2</v>
       </c>
@@ -451,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:9">
       <c r="B5">
         <v>3</v>
       </c>
@@ -471,7 +477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:9">
       <c r="B6">
         <v>4</v>
       </c>
@@ -491,7 +497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:9">
       <c r="B7">
         <v>5</v>
       </c>
@@ -511,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:9">
       <c r="B8">
         <v>6</v>
       </c>
@@ -531,7 +537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:9">
       <c r="B9">
         <v>7</v>
       </c>
@@ -551,7 +557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:9">
       <c r="B10">
         <v>8</v>
       </c>
@@ -571,7 +577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:9">
       <c r="B11">
         <v>9</v>
       </c>
@@ -591,7 +597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:9">
       <c r="B12">
         <v>10</v>
       </c>
@@ -611,7 +617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:9">
       <c r="B13">
         <v>11</v>
       </c>
@@ -631,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:9">
       <c r="B14">
         <v>12</v>
       </c>
@@ -651,7 +657,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:9">
       <c r="B15">
         <v>13</v>
       </c>
@@ -671,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:9">
       <c r="B16">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
repo1 again to doc
</commit_message>
<xml_diff>
--- a/Test/excel doc.xlsx
+++ b/Test/excel doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Column1</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>as</t>
+  </si>
+  <si>
+    <t>repo1</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -472,6 +475,9 @@
       </c>
       <c r="G4">
         <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9">

</xml_diff>

<commit_message>
repo 2 again to doc
</commit_message>
<xml_diff>
--- a/Test/excel doc.xlsx
+++ b/Test/excel doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Column1</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -471,6 +471,9 @@
         <v>6</v>
       </c>
       <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
repo 2 again to doc (reverse-merged from commit 936d68a3de6f404e571bd12710debc5260dcc67b)
</commit_message>
<xml_diff>
--- a/Test/excel doc.xlsx
+++ b/Test/excel doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Column1</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>as</t>
-  </si>
-  <si>
-    <t>repo1</t>
   </si>
 </sst>
 </file>
@@ -398,7 +395,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,9 +472,6 @@
       </c>
       <c r="G4">
         <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9">

</xml_diff>